<commit_message>
Version archivos 2 de junio de 2020
Version archivos 2 de junio de 2020
</commit_message>
<xml_diff>
--- a/2020/Directivos-colegio/Calculo nota de recuperacion.xlsx
+++ b/2020/Directivos-colegio/Calculo nota de recuperacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\Directivos-colegio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257DA4FD-2299-4B53-A630-E758C2D81E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E63D265-B2BB-4889-8979-E0514421ECD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="3090" windowWidth="14400" windowHeight="10755" xr2:uid="{51820E11-844B-4576-9580-A05F23FE2160}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{51820E11-844B-4576-9580-A05F23FE2160}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="6">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="6">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
       </c>
       <c r="C7" s="7">
         <f>ROUND((35-(B5%*C5+B6%*C6))/B7%, 0)</f>
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">

</xml_diff>